<commit_message>
Lab1 - Modified ReviewReport
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport_BigBelly.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport_BigBelly.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvelin\Desktop\FACULTA\VVSS\lab1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Faculta\Anul 3\Sem2\VVSS\VVSS_Inventory\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9659E6-8EF8-4948-815F-CF3930FD4EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7182FE-DED4-4384-928F-35C1D7BC5A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="13932" windowHeight="12336" tabRatio="650" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -230,25 +230,7 @@
     <t>Part, Product</t>
   </si>
   <si>
-    <t>Mesaje de eroare existente in validări.</t>
-  </si>
-  <si>
-    <t>C13</t>
-  </si>
-  <si>
-    <t>AddProductController, AddPartController</t>
-  </si>
-  <si>
-    <t>Câmpuri declarate, dar nu sunt folosite nicăieri</t>
-  </si>
-  <si>
     <t>C01</t>
-  </si>
-  <si>
-    <t>AddProductController, 138  ModifyProductController, 177 , Inventory, Product, InventoryRepository</t>
-  </si>
-  <si>
-    <t>Pentru ștergere nu e nevoie de obiect, ci de indicele lui.</t>
   </si>
   <si>
     <t>InventoryService, 46</t>
@@ -1312,6 +1294,24 @@
   </si>
   <si>
     <t>Velin Mihnea</t>
+  </si>
+  <si>
+    <t>Validarea inputului se face in service, nu in controller</t>
+  </si>
+  <si>
+    <t>Mesaje de eroare existente in validari.</t>
+  </si>
+  <si>
+    <t>C09</t>
+  </si>
+  <si>
+    <t>InventoryService 46,51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AddProductController 208,  AddPartController 155 </t>
+  </si>
+  <si>
+    <t>Utilizarea variabile partDynamicValue este ambigua</t>
   </si>
 </sst>
 </file>
@@ -1655,6 +1655,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1678,24 +1696,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2079,40 +2079,40 @@
   </sheetPr>
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="6"/>
+    <col min="10" max="10" width="14.44140625" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
       <c r="H2" s="3"/>
       <c r="I2" s="17" t="s">
         <v>30</v>
@@ -2126,7 +2126,7 @@
         <v>20</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="J3" s="16">
         <v>237</v>
@@ -2136,15 +2136,15 @@
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="44"/>
+      <c r="E4" s="36"/>
       <c r="H4" s="16" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="32" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J4" s="3">
         <v>237</v>
@@ -2154,15 +2154,15 @@
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="46"/>
+      <c r="E5" s="38"/>
       <c r="H5" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="32" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="J5" s="3">
         <v>237</v>
@@ -2173,15 +2173,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
@@ -2197,29 +2197,29 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="22.9" customHeight="1">
-      <c r="B10" s="39">
+    <row r="10" spans="1:10" ht="22.95" customHeight="1">
+      <c r="B10" s="45">
         <v>1</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="41" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="39" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="19.899999999999999" customHeight="1">
-      <c r="B11" s="40"/>
-      <c r="C11" s="36"/>
+    <row r="11" spans="1:10" ht="19.95" customHeight="1">
+      <c r="B11" s="46"/>
+      <c r="C11" s="42"/>
       <c r="D11" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="34"/>
-    </row>
-    <row r="12" spans="1:10" ht="45">
+      <c r="E11" s="40"/>
+    </row>
+    <row r="12" spans="1:10" ht="28.8">
       <c r="B12" s="22">
         <v>2</v>
       </c>
@@ -2234,48 +2234,48 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="B13" s="37">
+      <c r="B13" s="43">
         <v>3</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="41" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="39" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="B14" s="38"/>
-      <c r="C14" s="36"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="42"/>
       <c r="D14" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="34"/>
-    </row>
-    <row r="15" spans="1:10" ht="23.45" customHeight="1">
-      <c r="B15" s="39">
+      <c r="E14" s="40"/>
+    </row>
+    <row r="15" spans="1:10" ht="23.4" customHeight="1">
+      <c r="B15" s="45">
         <v>4</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="41" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="39" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="21" customHeight="1">
-      <c r="B16" s="40"/>
-      <c r="C16" s="36"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="42"/>
       <c r="D16" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="34"/>
+      <c r="E16" s="40"/>
     </row>
     <row r="17" spans="2:5" ht="30.6" customHeight="1">
       <c r="B17" s="22">
@@ -2302,12 +2302,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D5:E5"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="B13:B14"/>
@@ -2317,6 +2311,12 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2330,39 +2330,39 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
     <col min="9" max="9" width="22" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
       <c r="H2" s="3"/>
       <c r="I2" s="17" t="s">
         <v>30</v>
@@ -2376,7 +2376,7 @@
         <v>20</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="J3" s="16">
         <v>237</v>
@@ -2394,7 +2394,7 @@
         <v>21</v>
       </c>
       <c r="I4" s="32" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J4" s="3">
         <v>237</v>
@@ -2412,7 +2412,7 @@
         <v>22</v>
       </c>
       <c r="I5" s="32" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="J5" s="3">
         <v>237</v>
@@ -2423,15 +2423,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
@@ -2498,7 +2498,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="30">
+    <row r="14" spans="1:10" ht="28.8">
       <c r="B14" s="24">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2524,7 +2524,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="75">
+    <row r="16" spans="1:10" ht="72">
       <c r="B16" s="24">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2663,40 +2663,40 @@
   </sheetPr>
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="90.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
-    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="90.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
       <c r="H2" s="3"/>
       <c r="I2" s="17" t="s">
         <v>30</v>
@@ -2710,7 +2710,7 @@
         <v>20</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="J3" s="16">
         <v>237</v>
@@ -2728,7 +2728,7 @@
         <v>21</v>
       </c>
       <c r="I4" s="32" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J4" s="3">
         <v>237</v>
@@ -2746,7 +2746,7 @@
         <v>22</v>
       </c>
       <c r="I5" s="32" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="J5" s="3">
         <v>237</v>
@@ -2757,15 +2757,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
@@ -2792,28 +2792,28 @@
         <v>63</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="14.65" customHeight="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="14.7" customHeight="1">
       <c r="B11" s="29">
         <v>2</v>
       </c>
-      <c r="C11" s="35" t="s">
-        <v>65</v>
+      <c r="C11" s="41" t="s">
+        <v>101</v>
       </c>
       <c r="D11" s="55" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="B12" s="29">
         <v>3</v>
       </c>
-      <c r="C12" s="36"/>
+      <c r="C12" s="42"/>
       <c r="D12" s="57"/>
       <c r="E12" s="57"/>
     </row>
@@ -2821,19 +2821,19 @@
       <c r="B13" s="50">
         <v>4</v>
       </c>
-      <c r="C13" s="35" t="s">
-        <v>68</v>
+      <c r="C13" s="41" t="s">
+        <v>64</v>
       </c>
       <c r="D13" s="55" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="E13" s="55" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="87" customHeight="1">
       <c r="B14" s="51"/>
-      <c r="C14" s="36"/>
+      <c r="C14" s="42"/>
       <c r="D14" s="56"/>
       <c r="E14" s="57"/>
     </row>
@@ -2845,7 +2845,7 @@
       <c r="D15" s="26"/>
       <c r="E15" s="25"/>
     </row>
-    <row r="16" spans="1:10" ht="14.65" customHeight="1">
+    <row r="16" spans="1:10" ht="14.7" customHeight="1">
       <c r="B16" s="3">
         <f t="shared" ref="B16:B29" si="0">B15+1</f>
         <v>8</v>
@@ -3012,37 +3012,37 @@
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="59.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.7109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.85546875" style="6"/>
-    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="59.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.6640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="40.6640625" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
       <c r="H2" s="3"/>
       <c r="I2" s="17" t="s">
         <v>30</v>
@@ -3056,7 +3056,7 @@
         <v>20</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="J3" s="16">
         <v>237</v>
@@ -3072,7 +3072,7 @@
         <v>21</v>
       </c>
       <c r="I4" s="32" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J4" s="3">
         <v>237</v>
@@ -3082,13 +3082,13 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
       <c r="H5" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="32" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="J5" s="3">
         <v>237</v>
@@ -3099,8 +3099,8 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
       <c r="F6" s="18"/>
     </row>
     <row r="9" spans="1:10">
@@ -3120,21 +3120,21 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28.9" customHeight="1">
+    <row r="10" spans="1:10" ht="28.95" customHeight="1">
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D10" s="55" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F10" s="55" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3143,11 +3143,11 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D11" s="56"/>
       <c r="E11" s="30" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F11" s="56"/>
     </row>
@@ -3157,80 +3157,80 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D12" s="57"/>
       <c r="E12" s="30" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F12" s="57"/>
     </row>
-    <row r="13" spans="1:10" ht="60">
+    <row r="13" spans="1:10" ht="57.6">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="60">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="57.6">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D14" s="55" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="60">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="57.6">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D15" s="56"/>
       <c r="E15" s="31" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="75">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="57.6">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D16" s="57"/>
       <c r="E16" s="31" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="2:6">
@@ -3239,13 +3239,13 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F17" s="1"/>
     </row>
@@ -3255,16 +3255,16 @@
         <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F18" s="30" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="2:6">
@@ -3273,13 +3273,13 @@
         <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F19" s="2"/>
     </row>

</xml_diff>